<commit_message>
Add the TMCStepper library to enable controlling the features of the TMC2209 like CoolStep to save 75% energy and StealthChop to make the stepper motors silent at low speed. Replace the LED logic with one that uses the I2S to drive WS2812 addressable LEDs Update JTAG debugging documentation
</commit_message>
<xml_diff>
--- a/Related chip information/ESP32 pin assignments.xlsx
+++ b/Related chip information/ESP32 pin assignments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\ada\Related chip information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4AF7675-7A54-4223-BDF7-B1AEBD557B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3E8E7C-B415-4129-9E57-5A71D4EE7E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="8490" windowWidth="25440" windowHeight="15270" xr2:uid="{56C63F47-42D5-4463-8DA8-24EC799EC9D3}"/>
+    <workbookView xWindow="25695" yWindow="-15" windowWidth="26010" windowHeight="20985" xr2:uid="{56C63F47-42D5-4463-8DA8-24EC799EC9D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="120">
   <si>
     <t>Vin 5V</t>
   </si>
@@ -215,16 +215,7 @@
     <t>outputs PWM signal at boot</t>
   </si>
   <si>
-    <t>MPU_INTERRUPT</t>
-  </si>
-  <si>
     <t>Ada assignment</t>
-  </si>
-  <si>
-    <t>VIN_5V</t>
-  </si>
-  <si>
-    <t>VOUT_3.3V</t>
   </si>
   <si>
     <t>JTAG 2 (TMS)</t>
@@ -393,12 +384,36 @@
   <si>
     <t>RX2</t>
   </si>
+  <si>
+    <t>TMC2209 right uStep Pin1</t>
+  </si>
+  <si>
+    <t>LED I2S output</t>
+  </si>
+  <si>
+    <t>MPU_6050 Interrupt</t>
+  </si>
+  <si>
+    <t>JTAG VDD</t>
+  </si>
+  <si>
+    <t>JTAG GND</t>
+  </si>
+  <si>
+    <t>VIN_3.3V</t>
+  </si>
+  <si>
+    <t>Battery Voltage</t>
+  </si>
+  <si>
+    <t>TMC2209 right uStep Pin2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -446,8 +461,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -469,24 +492,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -561,7 +566,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -575,20 +580,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -603,7 +605,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -612,11 +614,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1126,7 +1129,7 @@
   <dimension ref="B2:L62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1138,34 +1141,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12">
-      <c r="B2" t="s">
+      <c r="B2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E2" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" s="20"/>
+      <c r="H2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="K2" t="s">
-        <v>60</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="K2" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" s="20" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1176,7 +1180,7 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>117</v>
       </c>
       <c r="H3" t="s">
         <v>14</v>
@@ -1200,6 +1204,9 @@
       <c r="J4" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="K4" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="5" spans="2:12">
       <c r="B5" t="s">
@@ -1211,6 +1218,9 @@
       <c r="D5" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="E5" s="17" t="s">
+        <v>118</v>
+      </c>
       <c r="F5" t="s">
         <v>48</v>
       </c>
@@ -1222,7 +1232,7 @@
       </c>
       <c r="J5" s="4"/>
       <c r="K5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="2:12">
@@ -1235,6 +1245,7 @@
       <c r="D6" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="E6" s="17"/>
       <c r="F6" t="s">
         <v>48</v>
       </c>
@@ -1242,11 +1253,12 @@
         <v>26</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="K6" s="17"/>
       <c r="L6" t="s">
         <v>55</v>
       </c>
@@ -1261,6 +1273,7 @@
       <c r="D7" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="E7" s="17"/>
       <c r="F7" t="s">
         <v>48</v>
       </c>
@@ -1271,8 +1284,9 @@
         <v>23</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>112</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="K7" s="17"/>
       <c r="L7" t="s">
         <v>54</v>
       </c>
@@ -1287,6 +1301,7 @@
       <c r="D8" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="E8" s="17"/>
       <c r="F8" t="s">
         <v>48</v>
       </c>
@@ -1298,7 +1313,7 @@
       </c>
       <c r="J8" s="4"/>
       <c r="K8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="2:12">
@@ -1312,7 +1327,7 @@
         <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H9" t="s">
         <v>14</v>
@@ -1332,7 +1347,7 @@
         <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H10" t="s">
         <v>29</v>
@@ -1343,8 +1358,8 @@
       <c r="J10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K10" s="20" t="s">
-        <v>110</v>
+      <c r="K10" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="2:12">
@@ -1358,7 +1373,7 @@
         <v>23</v>
       </c>
       <c r="E11" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H11" t="s">
         <v>30</v>
@@ -1369,8 +1384,8 @@
       <c r="J11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="20" t="s">
-        <v>108</v>
+      <c r="K11" s="19" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="2:12">
@@ -1384,7 +1399,7 @@
         <v>23</v>
       </c>
       <c r="E12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H12" t="s">
         <v>31</v>
@@ -1395,8 +1410,8 @@
       <c r="J12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K12" s="20" t="s">
-        <v>109</v>
+      <c r="K12" s="19" t="s">
+        <v>106</v>
       </c>
       <c r="L12" t="s">
         <v>53</v>
@@ -1412,20 +1427,20 @@
       <c r="D13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="22" t="s">
-        <v>110</v>
+      <c r="E13" s="19" t="s">
+        <v>119</v>
       </c>
       <c r="H13" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="21" t="s">
-        <v>113</v>
+      <c r="I13" s="18" t="s">
+        <v>110</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K13" t="s">
-        <v>101</v>
+      <c r="K13" s="19" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="2:12">
@@ -1439,7 +1454,7 @@
         <v>44</v>
       </c>
       <c r="E14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F14" t="s">
         <v>58</v>
@@ -1450,11 +1465,11 @@
       <c r="I14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J14" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="K14" t="s">
-        <v>102</v>
+      <c r="J14" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="K14" s="19" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="2:12">
@@ -1467,8 +1482,8 @@
       <c r="D15" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>64</v>
+      <c r="E15" s="19" t="s">
+        <v>61</v>
       </c>
       <c r="F15" t="s">
         <v>57</v>
@@ -1481,6 +1496,9 @@
       </c>
       <c r="J15" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="K15" s="19" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="2:12">
@@ -1490,7 +1508,7 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="H16" t="s">
         <v>35</v>
@@ -1501,6 +1519,7 @@
       <c r="J16" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="K16" s="17"/>
       <c r="L16" t="s">
         <v>51</v>
       </c>
@@ -1515,8 +1534,8 @@
       <c r="D17" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>65</v>
+      <c r="E17" s="19" t="s">
+        <v>62</v>
       </c>
       <c r="H17" t="s">
         <v>36</v>
@@ -1527,8 +1546,8 @@
       <c r="J17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K17" t="s">
-        <v>59</v>
+      <c r="K17" s="17" t="s">
+        <v>113</v>
       </c>
       <c r="L17" t="s">
         <v>56</v>
@@ -1556,8 +1575,8 @@
       <c r="J18" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="K18" s="7" t="s">
-        <v>66</v>
+      <c r="K18" s="19" t="s">
+        <v>63</v>
       </c>
       <c r="L18" t="s">
         <v>53</v>
@@ -1622,7 +1641,7 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" t="s">
-        <v>61</v>
+        <v>115</v>
       </c>
       <c r="H21" t="s">
         <v>40</v>
@@ -1638,281 +1657,281 @@
       </c>
     </row>
     <row r="24" spans="2:12">
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" ht="181.5" customHeight="1">
+      <c r="C25" s="11"/>
+    </row>
+    <row r="26" spans="2:12" ht="16.5" thickBot="1">
+      <c r="C26" s="5"/>
+    </row>
+    <row r="27" spans="2:12" ht="86.25" thickBot="1">
+      <c r="C27" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" s="12" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="25" spans="2:12" ht="181.5" customHeight="1">
-      <c r="C25" s="14"/>
-    </row>
-    <row r="26" spans="2:12" ht="16.5" thickBot="1">
-      <c r="C26" s="8"/>
-    </row>
-    <row r="27" spans="2:12" ht="86.25" thickBot="1">
-      <c r="C27" s="15" t="s">
+      <c r="F27" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D27" s="15" t="s">
+    </row>
+    <row r="28" spans="2:12" ht="15.75" thickBot="1">
+      <c r="C28" s="7">
+        <v>1</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E28" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F28" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="F27" s="16" t="s">
+    </row>
+    <row r="29" spans="2:12" ht="15.75" thickBot="1">
+      <c r="C29" s="8">
+        <v>3</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="15" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="2:12" ht="15.75" thickBot="1">
-      <c r="C28" s="10">
+    <row r="30" spans="2:12" ht="15.75" thickBot="1">
+      <c r="C30" s="7">
+        <v>2</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" ht="15.75" thickBot="1">
+      <c r="C31" s="8">
+        <v>4</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" ht="15.75" thickBot="1">
+      <c r="C32" s="7">
+        <v>6</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" ht="15.75" thickBot="1">
+      <c r="C33" s="8">
+        <v>8</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" ht="23.25">
+      <c r="B54" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" ht="16.5" thickBot="1">
+      <c r="B55" s="5"/>
+    </row>
+    <row r="56" spans="2:8" ht="86.25" thickBot="1">
+      <c r="B56" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="H56" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" ht="171.75" thickBot="1">
+      <c r="B57" s="7">
         <v>1</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="C57" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H57" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" ht="29.25" thickBot="1">
+      <c r="B58" s="8">
+        <v>3</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G58" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H58" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" ht="43.5" thickBot="1">
+      <c r="B59" s="7">
+        <v>2</v>
+      </c>
+      <c r="C59" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E28" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F28" s="17" t="s">
+      <c r="D59" s="7" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="29" spans="2:12" ht="15.75" thickBot="1">
-      <c r="C29" s="11">
-        <v>3</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" s="18" t="s">
+      <c r="E59" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H59" s="9" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="2:12" ht="15.75" thickBot="1">
-      <c r="C30" s="10">
-        <v>2</v>
-      </c>
-      <c r="D30" s="10" t="s">
+    <row r="60" spans="2:8" ht="57.75" thickBot="1">
+      <c r="B60" s="8">
+        <v>4</v>
+      </c>
+      <c r="C60" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="D60" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="F30" s="17" t="s">
+      <c r="E60" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G60" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="H60" s="10" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="2:12" ht="15.75" thickBot="1">
-      <c r="C31" s="11">
-        <v>4</v>
-      </c>
-      <c r="D31" s="11" t="s">
+    <row r="61" spans="2:8" ht="43.5" thickBot="1">
+      <c r="B61" s="7">
+        <v>6</v>
+      </c>
+      <c r="C61" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="D61" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F31" s="18" t="s">
+      <c r="E61" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="H61" s="9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="2:12" ht="15.75" thickBot="1">
-      <c r="C32" s="10">
-        <v>6</v>
-      </c>
-      <c r="D32" s="10" t="s">
+    <row r="62" spans="2:8" ht="29.25" thickBot="1">
+      <c r="B62" s="8">
+        <v>8</v>
+      </c>
+      <c r="C62" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="D62" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="F32" s="17" t="s">
+      <c r="E62" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F62" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="G62" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H62" s="10" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6" ht="15.75" thickBot="1">
-      <c r="C33" s="11">
-        <v>8</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="F33" s="18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8" ht="23.25">
-      <c r="B54" s="14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" ht="16.5" thickBot="1">
-      <c r="B55" s="8"/>
-    </row>
-    <row r="56" spans="2:8" ht="86.25" thickBot="1">
-      <c r="B56" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D56" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E56" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="F56" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="G56" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="H56" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8" ht="171.75" thickBot="1">
-      <c r="B57" s="10">
-        <v>1</v>
-      </c>
-      <c r="C57" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D57" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E57" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F57" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="G57" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="H57" s="12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8" ht="29.25" thickBot="1">
-      <c r="B58" s="11">
-        <v>3</v>
-      </c>
-      <c r="C58" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D58" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E58" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F58" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G58" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H58" s="13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="59" spans="2:8" ht="43.5" thickBot="1">
-      <c r="B59" s="10">
-        <v>2</v>
-      </c>
-      <c r="C59" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D59" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="E59" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="F59" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="G59" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="H59" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="60" spans="2:8" ht="57.75" thickBot="1">
-      <c r="B60" s="11">
-        <v>4</v>
-      </c>
-      <c r="C60" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D60" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E60" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="F60" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="G60" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="H60" s="13" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8" ht="43.5" thickBot="1">
-      <c r="B61" s="10">
-        <v>6</v>
-      </c>
-      <c r="C61" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="D61" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E61" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F61" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="G61" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="H61" s="12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="62" spans="2:8" ht="29.25" thickBot="1">
-      <c r="B62" s="11">
-        <v>8</v>
-      </c>
-      <c r="C62" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="D62" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E62" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="F62" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="G62" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="H62" s="13" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove more dead code and variables to improve readability of the code Switch boolean values to use true/false to improve readability of the code Clean up and document Expodential Smoothing code, variable names and comments (flip to the more standard algorythm) Update EasyEDA Pro schematic design  - shorten board by placing power supply under ESP32  - remove header pins by TMC2209 as they are no longer needed  - add simple amplifier circuit just to see if I can make it fit
</commit_message>
<xml_diff>
--- a/Related chip information/ESP32 pin assignments.xlsx
+++ b/Related chip information/ESP32 pin assignments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\ada\Related chip information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3E8E7C-B415-4129-9E57-5A71D4EE7E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE4C7A6-56DA-4F1D-A211-EB45C68AADB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="-15" windowWidth="26010" windowHeight="20985" xr2:uid="{56C63F47-42D5-4463-8DA8-24EC799EC9D3}"/>
+    <workbookView xWindow="15030" yWindow="75" windowWidth="10170" windowHeight="14955" xr2:uid="{56C63F47-42D5-4463-8DA8-24EC799EC9D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="122">
   <si>
     <t>Vin 5V</t>
   </si>
@@ -407,6 +407,12 @@
   </si>
   <si>
     <t>TMC2209 right uStep Pin2</t>
+  </si>
+  <si>
+    <t>DAC_RIGHT</t>
+  </si>
+  <si>
+    <t>DAC_LEFT</t>
   </si>
 </sst>
 </file>
@@ -470,7 +476,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -510,6 +516,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -566,7 +584,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -618,8 +636,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -642,13 +661,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>47626</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>171451</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>76201</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>151040</xdr:rowOff>
@@ -686,13 +705,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>1581150</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>1666875</xdr:rowOff>
@@ -747,13 +766,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>29584</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>1257299</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -1126,682 +1145,688 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F3D7790-DAF5-429B-A1FC-5D7BE5EFA8F6}">
-  <dimension ref="B2:L62"/>
+  <dimension ref="B2:M62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="F12" sqref="F12:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22" customWidth="1"/>
-    <col min="12" max="12" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22" customWidth="1"/>
+    <col min="13" max="13" width="33.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12">
-      <c r="B2" s="20" t="s">
+    <row r="2" spans="2:13">
+      <c r="C2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="D2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="E2" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="F2" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="G2" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="19"/>
+      <c r="I2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="J2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="K2" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="L2" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="M2" s="19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="2:12">
-      <c r="B3" t="s">
+    <row r="3" spans="2:13">
+      <c r="C3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" t="s">
+      <c r="E3" s="2"/>
+      <c r="F3" t="s">
         <v>117</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>14</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:12">
-      <c r="B4" t="s">
+    <row r="4" spans="2:13">
+      <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="H4" t="s">
+      <c r="E4" s="2"/>
+      <c r="I4" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="J4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="2:12">
-      <c r="B5" t="s">
+    <row r="5" spans="2:13">
+      <c r="C5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="F5" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>48</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="K5" t="s">
+      <c r="K5" s="4"/>
+      <c r="L5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="2:12">
-      <c r="B6" t="s">
+    <row r="6" spans="2:13">
+      <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="17"/>
-      <c r="F6" t="s">
+      <c r="F6" s="17"/>
+      <c r="G6" t="s">
         <v>48</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="J6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" s="17"/>
-      <c r="L6" t="s">
+      <c r="K6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="17"/>
+      <c r="M6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="2:12">
-      <c r="B7" t="s">
+    <row r="7" spans="2:13">
+      <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" t="s">
+      <c r="F7" s="17"/>
+      <c r="G7" t="s">
         <v>48</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="K7" s="17"/>
-      <c r="L7" t="s">
+      <c r="L7" s="17"/>
+      <c r="M7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="2:12">
-      <c r="B8" t="s">
+    <row r="8" spans="2:13">
+      <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="17"/>
-      <c r="F8" t="s">
+      <c r="F8" s="17"/>
+      <c r="G8" t="s">
         <v>48</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="J8" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="J8" s="4"/>
-      <c r="K8" t="s">
+      <c r="K8" s="4"/>
+      <c r="L8" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="2:12">
-      <c r="B9" t="s">
+    <row r="9" spans="2:13">
+      <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="D9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
         <v>101</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>14</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:12">
-      <c r="B10" t="s">
+    <row r="10" spans="2:13">
+      <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="D10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" t="s">
         <v>102</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="J10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="2:12">
-      <c r="B11" t="s">
+    <row r="11" spans="2:13">
+      <c r="B11" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="D11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" t="s">
         <v>103</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="J11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="19" t="s">
+      <c r="K11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="2:12">
-      <c r="B12" t="s">
+    <row r="12" spans="2:13">
+      <c r="B12" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="D12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>31</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="J12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K12" s="19" t="s">
+      <c r="K12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" t="s">
         <v>106</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="2:12">
-      <c r="B13" t="s">
+    <row r="13" spans="2:13">
+      <c r="C13" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="D13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="18" t="s">
+      <c r="J13" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K13" s="19" t="s">
+      <c r="K13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="2:12">
-      <c r="B14" t="s">
+    <row r="14" spans="2:13">
+      <c r="C14" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>60</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>58</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>33</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J14" s="18" t="s">
+      <c r="J14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="K14" s="19" t="s">
+      <c r="L14" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="2:12">
-      <c r="B15" t="s">
+    <row r="15" spans="2:13">
+      <c r="C15" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="F15" t="s">
         <v>61</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>57</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>34</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="J15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K15" s="19" t="s">
+      <c r="K15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L15" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="2:12">
-      <c r="B16" t="s">
+    <row r="16" spans="2:13">
+      <c r="C16" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="E16" t="s">
+      <c r="E16" s="2"/>
+      <c r="F16" t="s">
         <v>116</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>35</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="J16" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K16" s="17"/>
-      <c r="L16" t="s">
+      <c r="K16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L16" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="M16" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="2:12">
-      <c r="B17" t="s">
+    <row r="17" spans="3:13">
+      <c r="C17" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="F17" t="s">
         <v>62</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>36</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="J17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K17" s="17" t="s">
+      <c r="K17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L17" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="2:12">
-      <c r="B18" t="s">
+    <row r="18" spans="3:13">
+      <c r="C18" t="s">
         <v>16</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F18" t="s">
+      <c r="E18" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" t="s">
         <v>42</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>37</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="J18" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="K18" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="K18" s="19" t="s">
+      <c r="L18" t="s">
         <v>63</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="2:12">
-      <c r="B19" t="s">
+    <row r="19" spans="3:13">
+      <c r="C19" t="s">
         <v>17</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F19" t="s">
+      <c r="E19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" t="s">
         <v>42</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>38</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="L19" t="s">
+      <c r="K19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M19" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="2:12">
-      <c r="B20" t="s">
+    <row r="20" spans="3:13">
+      <c r="C20" t="s">
         <v>18</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F20" t="s">
+      <c r="E20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" t="s">
         <v>42</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>39</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="L20" t="s">
+      <c r="K20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M20" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="2:12">
-      <c r="B21" t="s">
+    <row r="21" spans="3:13">
+      <c r="C21" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" t="s">
+      <c r="E21" s="2"/>
+      <c r="F21" t="s">
         <v>115</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>40</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="L21" t="s">
+      <c r="K21" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="2:12">
-      <c r="C24" s="16" t="s">
+    <row r="24" spans="3:13">
+      <c r="D24" s="16" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="2:12" ht="181.5" customHeight="1">
-      <c r="C25" s="11"/>
-    </row>
-    <row r="26" spans="2:12" ht="16.5" thickBot="1">
-      <c r="C26" s="5"/>
-    </row>
-    <row r="27" spans="2:12" ht="86.25" thickBot="1">
-      <c r="C27" s="12" t="s">
+    <row r="25" spans="3:13" ht="181.5" customHeight="1">
+      <c r="D25" s="11"/>
+    </row>
+    <row r="26" spans="3:13" ht="16.5" thickBot="1">
+      <c r="D26" s="5"/>
+    </row>
+    <row r="27" spans="3:13" ht="86.25" thickBot="1">
+      <c r="D27" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="E27" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="F27" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="G27" s="13" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="2:12" ht="15.75" thickBot="1">
-      <c r="C28" s="7">
+    <row r="28" spans="3:13" ht="15.75" thickBot="1">
+      <c r="D28" s="7">
         <v>1</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>69</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="F28" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G28" s="14" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="2:12" ht="15.75" thickBot="1">
-      <c r="C29" s="8">
+    <row r="29" spans="3:13" ht="15.75" thickBot="1">
+      <c r="D29" s="8">
         <v>3</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F29" s="15" t="s">
+      <c r="F29" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="15" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="2:12" ht="15.75" thickBot="1">
-      <c r="C30" s="7">
+    <row r="30" spans="3:13" ht="15.75" thickBot="1">
+      <c r="D30" s="7">
         <v>2</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="E30" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="F30" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="F30" s="14" t="s">
+      <c r="G30" s="14" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="2:12" ht="15.75" thickBot="1">
-      <c r="C31" s="8">
+    <row r="31" spans="3:13" ht="15.75" thickBot="1">
+      <c r="D31" s="8">
         <v>4</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="E31" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="F31" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="F31" s="15" t="s">
+      <c r="G31" s="15" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="2:12" ht="15.75" thickBot="1">
-      <c r="C32" s="7">
+    <row r="32" spans="3:13" ht="15.75" thickBot="1">
+      <c r="D32" s="7">
         <v>6</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="E32" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="F32" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F32" s="14" t="s">
+      <c r="G32" s="14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="3:6" ht="15.75" thickBot="1">
-      <c r="C33" s="8">
+    <row r="33" spans="4:7" ht="15.75" thickBot="1">
+      <c r="D33" s="8">
         <v>8</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="E33" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="F33" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="F33" s="15" t="s">
+      <c r="G33" s="15" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="54" spans="2:8" ht="23.25">
-      <c r="B54" s="11" t="s">
+    <row r="54" spans="3:9" ht="23.25">
+      <c r="C54" s="11" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="2:8" ht="16.5" thickBot="1">
-      <c r="B55" s="5"/>
-    </row>
-    <row r="56" spans="2:8" ht="86.25" thickBot="1">
-      <c r="B56" s="6" t="s">
+    <row r="55" spans="3:9" ht="16.5" thickBot="1">
+      <c r="C55" s="5"/>
+    </row>
+    <row r="56" spans="3:9" ht="86.25" thickBot="1">
+      <c r="C56" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="D56" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D56" s="6" t="s">
+      <c r="E56" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E56" s="6" t="s">
+      <c r="F56" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="F56" s="6" t="s">
+      <c r="G56" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="G56" s="6" t="s">
+      <c r="H56" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="H56" s="6" t="s">
+      <c r="I56" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="2:8" ht="171.75" thickBot="1">
-      <c r="B57" s="7">
+    <row r="57" spans="3:9" ht="171.75" thickBot="1">
+      <c r="C57" s="7">
         <v>1</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>69</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>69</v>
@@ -1815,16 +1840,16 @@
       <c r="G57" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="H57" s="9" t="s">
+      <c r="H57" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I57" s="9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="2:8" ht="29.25" thickBot="1">
-      <c r="B58" s="8">
+    <row r="58" spans="3:9" ht="29.25" thickBot="1">
+      <c r="C58" s="8">
         <v>3</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="D58" s="8" t="s">
         <v>14</v>
@@ -1838,105 +1863,108 @@
       <c r="G58" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H58" s="10" t="s">
+      <c r="H58" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I58" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="2:8" ht="43.5" thickBot="1">
-      <c r="B59" s="7">
+    <row r="59" spans="3:9" ht="43.5" thickBot="1">
+      <c r="C59" s="7">
         <v>2</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="D59" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D59" s="7" t="s">
+      <c r="E59" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E59" s="7" t="s">
+      <c r="F59" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F59" s="7" t="s">
+      <c r="G59" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="G59" s="7" t="s">
+      <c r="H59" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="H59" s="9" t="s">
+      <c r="I59" s="9" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="60" spans="2:8" ht="57.75" thickBot="1">
-      <c r="B60" s="8">
+    <row r="60" spans="3:9" ht="57.75" thickBot="1">
+      <c r="C60" s="8">
         <v>4</v>
       </c>
-      <c r="C60" s="8" t="s">
+      <c r="D60" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D60" s="8" t="s">
+      <c r="E60" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="E60" s="8" t="s">
+      <c r="F60" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="F60" s="8" t="s">
+      <c r="G60" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="G60" s="8" t="s">
+      <c r="H60" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="H60" s="10" t="s">
+      <c r="I60" s="10" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="61" spans="2:8" ht="43.5" thickBot="1">
-      <c r="B61" s="7">
+    <row r="61" spans="3:9" ht="43.5" thickBot="1">
+      <c r="C61" s="7">
         <v>6</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="D61" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="E61" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E61" s="7" t="s">
+      <c r="F61" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F61" s="7" t="s">
+      <c r="G61" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G61" s="7" t="s">
+      <c r="H61" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="H61" s="9" t="s">
+      <c r="I61" s="9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="62" spans="2:8" ht="29.25" thickBot="1">
-      <c r="B62" s="8">
+    <row r="62" spans="3:9" ht="29.25" thickBot="1">
+      <c r="C62" s="8">
         <v>8</v>
       </c>
-      <c r="C62" s="8" t="s">
+      <c r="D62" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D62" s="8" t="s">
+      <c r="E62" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E62" s="8" t="s">
+      <c r="F62" s="8" t="s">
         <v>96</v>
-      </c>
-      <c r="F62" s="8" t="s">
-        <v>97</v>
       </c>
       <c r="G62" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="H62" s="10" t="s">
+      <c r="H62" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="I62" s="10" t="s">
         <v>83</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C24" r:id="rId1" location="debugging-tool-esp-prog" xr:uid="{167A5285-DC89-488D-9FCD-3AA8657AEDB3}"/>
+    <hyperlink ref="D24" r:id="rId1" location="debugging-tool-esp-prog" xr:uid="{167A5285-DC89-488D-9FCD-3AA8657AEDB3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Update Ada EasyEDAPro file with the V2 hardware design. Update the #SP32 pin assignments to match the V2 hardware. Update the (unused) Amplifier Design Notes.
</commit_message>
<xml_diff>
--- a/Related chip information/ESP32 pin assignments.xlsx
+++ b/Related chip information/ESP32 pin assignments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\ada\Related chip information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE4C7A6-56DA-4F1D-A211-EB45C68AADB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D36706-12CE-43DF-9B77-2F24978DA303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15030" yWindow="75" windowWidth="10170" windowHeight="14955" xr2:uid="{56C63F47-42D5-4463-8DA8-24EC799EC9D3}"/>
+    <workbookView xWindow="51480" yWindow="8490" windowWidth="25440" windowHeight="15270" xr2:uid="{56C63F47-42D5-4463-8DA8-24EC799EC9D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="121">
   <si>
     <t>Vin 5V</t>
   </si>
@@ -352,18 +352,6 @@
     <t>MPU_6050 I2C</t>
   </si>
   <si>
-    <t>TMC2209 left dir pin (UART 0)</t>
-  </si>
-  <si>
-    <t>TMC2209 left step pin (UART 0)</t>
-  </si>
-  <si>
-    <t>TMC2209 right dir  pin (UART 1)</t>
-  </si>
-  <si>
-    <t>TMC2209 right step pin (UART 1)</t>
-  </si>
-  <si>
     <t>TMC2209 left uStep Pin1</t>
   </si>
   <si>
@@ -400,9 +388,6 @@
     <t>JTAG GND</t>
   </si>
   <si>
-    <t>VIN_3.3V</t>
-  </si>
-  <si>
     <t>Battery Voltage</t>
   </si>
   <si>
@@ -413,6 +398,18 @@
   </si>
   <si>
     <t>DAC_LEFT</t>
+  </si>
+  <si>
+    <t>TMC2209 right dir pin (UART 0)</t>
+  </si>
+  <si>
+    <t>TMC2209 right step pin (UART 0)</t>
+  </si>
+  <si>
+    <t>TMC2209 left dir  pin (UART 1)</t>
+  </si>
+  <si>
+    <t>TMC2209 left step pin (UART 1)</t>
   </si>
 </sst>
 </file>
@@ -476,7 +473,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -509,12 +506,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -527,7 +518,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -584,7 +575,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -632,13 +623,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1145,62 +1137,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F3D7790-DAF5-429B-A1FC-5D7BE5EFA8F6}">
-  <dimension ref="B2:M62"/>
+  <dimension ref="A2:M62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12:F13"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="33.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22" customWidth="1"/>
     <col min="13" max="13" width="33.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13">
-      <c r="C2" s="19" t="s">
+    <row r="2" spans="1:13">
+      <c r="C2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19" t="s">
+      <c r="H2" s="18"/>
+      <c r="I2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="K2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="19" t="s">
+      <c r="L2" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="M2" s="19" t="s">
+      <c r="M2" s="18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="2:13">
+    <row r="3" spans="1:13">
+      <c r="B3">
+        <v>1</v>
+      </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" t="s">
-        <v>117</v>
+      <c r="F3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
       </c>
       <c r="I3" t="s">
         <v>14</v>
@@ -1209,12 +1207,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:13">
+    <row r="4" spans="1:13">
+      <c r="B4">
+        <v>2</v>
+      </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
       <c r="I4" t="s">
         <v>24</v>
       </c>
@@ -1225,10 +1232,13 @@
         <v>23</v>
       </c>
       <c r="L4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="B5">
+        <v>3</v>
+      </c>
       <c r="C5" t="s">
         <v>3</v>
       </c>
@@ -1238,11 +1248,14 @@
       <c r="E5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="17" t="s">
-        <v>118</v>
+      <c r="F5" t="s">
+        <v>113</v>
       </c>
       <c r="G5" t="s">
         <v>48</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
       </c>
       <c r="I5" t="s">
         <v>25</v>
@@ -1255,7 +1268,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="2:13">
+    <row r="6" spans="1:13">
+      <c r="B6">
+        <v>4</v>
+      </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
@@ -1265,25 +1281,35 @@
       <c r="E6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="17"/>
+      <c r="F6" s="20" t="s">
+        <v>41</v>
+      </c>
       <c r="G6" t="s">
         <v>48</v>
       </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
       <c r="I6" t="s">
         <v>26</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L6" s="17"/>
+      <c r="L6" s="20" t="s">
+        <v>41</v>
+      </c>
       <c r="M6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="2:13">
+    <row r="7" spans="1:13">
+      <c r="B7">
+        <v>5</v>
+      </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
@@ -1293,10 +1319,15 @@
       <c r="E7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="17"/>
+      <c r="F7" s="20" t="s">
+        <v>41</v>
+      </c>
       <c r="G7" t="s">
         <v>48</v>
       </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
       <c r="I7" t="s">
         <v>27</v>
       </c>
@@ -1304,14 +1335,19 @@
         <v>23</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="L7" s="17"/>
+        <v>105</v>
+      </c>
+      <c r="L7" s="20" t="s">
+        <v>41</v>
+      </c>
       <c r="M7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="2:13">
+    <row r="8" spans="1:13">
+      <c r="B8">
+        <v>6</v>
+      </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
@@ -1321,9 +1357,14 @@
       <c r="E8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="17"/>
+      <c r="F8" s="20" t="s">
+        <v>41</v>
+      </c>
       <c r="G8" t="s">
         <v>48</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
       </c>
       <c r="I8" t="s">
         <v>28</v>
@@ -1336,7 +1377,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="2:13">
+    <row r="9" spans="1:13">
+      <c r="B9">
+        <v>7</v>
+      </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
@@ -1347,7 +1391,10 @@
         <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>101</v>
+        <v>117</v>
+      </c>
+      <c r="H9">
+        <v>7</v>
       </c>
       <c r="I9" t="s">
         <v>14</v>
@@ -1356,7 +1403,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:13">
+    <row r="10" spans="1:13">
+      <c r="B10">
+        <v>8</v>
+      </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
@@ -1367,7 +1417,10 @@
         <v>23</v>
       </c>
       <c r="F10" t="s">
-        <v>102</v>
+        <v>118</v>
+      </c>
+      <c r="H10">
+        <v>8</v>
       </c>
       <c r="I10" t="s">
         <v>29</v>
@@ -1379,12 +1432,15 @@
         <v>23</v>
       </c>
       <c r="L10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13">
-      <c r="B11" s="20" t="s">
-        <v>120</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -1396,7 +1452,10 @@
         <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>103</v>
+        <v>119</v>
+      </c>
+      <c r="H11">
+        <v>9</v>
       </c>
       <c r="I11" t="s">
         <v>30</v>
@@ -1408,12 +1467,15 @@
         <v>23</v>
       </c>
       <c r="L11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13">
-      <c r="B12" s="20" t="s">
-        <v>121</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -1424,8 +1486,11 @@
       <c r="E12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="21" t="s">
-        <v>104</v>
+      <c r="F12" t="s">
+        <v>120</v>
+      </c>
+      <c r="H12">
+        <v>10</v>
       </c>
       <c r="I12" t="s">
         <v>31</v>
@@ -1437,13 +1502,16 @@
         <v>23</v>
       </c>
       <c r="L12" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="M12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="2:13">
+    <row r="13" spans="1:13">
+      <c r="B13">
+        <v>11</v>
+      </c>
       <c r="C13" t="s">
         <v>11</v>
       </c>
@@ -1453,14 +1521,17 @@
       <c r="E13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="21" t="s">
-        <v>119</v>
+      <c r="F13" t="s">
+        <v>103</v>
+      </c>
+      <c r="H13">
+        <v>11</v>
       </c>
       <c r="I13" t="s">
         <v>32</v>
       </c>
-      <c r="J13" s="18" t="s">
-        <v>110</v>
+      <c r="J13" s="17" t="s">
+        <v>106</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>23</v>
@@ -1469,7 +1540,10 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="2:13">
+    <row r="14" spans="1:13">
+      <c r="B14">
+        <v>12</v>
+      </c>
       <c r="C14" t="s">
         <v>12</v>
       </c>
@@ -1485,20 +1559,26 @@
       <c r="G14" t="s">
         <v>58</v>
       </c>
+      <c r="H14">
+        <v>12</v>
+      </c>
       <c r="I14" t="s">
         <v>33</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K14" s="18" t="s">
-        <v>111</v>
+      <c r="K14" s="17" t="s">
+        <v>107</v>
       </c>
       <c r="L14" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="2:13">
+    <row r="15" spans="1:13">
+      <c r="B15">
+        <v>13</v>
+      </c>
       <c r="C15" t="s">
         <v>13</v>
       </c>
@@ -1514,6 +1594,9 @@
       <c r="G15" t="s">
         <v>57</v>
       </c>
+      <c r="H15">
+        <v>13</v>
+      </c>
       <c r="I15" t="s">
         <v>34</v>
       </c>
@@ -1524,17 +1607,23 @@
         <v>23</v>
       </c>
       <c r="L15" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="B16">
+        <v>14</v>
+      </c>
       <c r="C16" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" t="s">
-        <v>116</v>
+        <v>112</v>
+      </c>
+      <c r="H16">
+        <v>14</v>
       </c>
       <c r="I16" t="s">
         <v>35</v>
@@ -1545,14 +1634,17 @@
       <c r="K16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L16" s="21" t="s">
-        <v>119</v>
+      <c r="L16" s="20" t="s">
+        <v>41</v>
       </c>
       <c r="M16" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="3:13">
+    <row r="17" spans="2:13">
+      <c r="B17">
+        <v>15</v>
+      </c>
       <c r="C17" t="s">
         <v>15</v>
       </c>
@@ -1565,6 +1657,9 @@
       <c r="F17" t="s">
         <v>62</v>
       </c>
+      <c r="H17">
+        <v>15</v>
+      </c>
       <c r="I17" t="s">
         <v>36</v>
       </c>
@@ -1574,14 +1669,17 @@
       <c r="K17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L17" s="17" t="s">
-        <v>113</v>
+      <c r="L17" t="s">
+        <v>109</v>
       </c>
       <c r="M17" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="3:13">
+    <row r="18" spans="2:13">
+      <c r="B18">
+        <v>16</v>
+      </c>
       <c r="C18" t="s">
         <v>16</v>
       </c>
@@ -1591,9 +1689,15 @@
       <c r="E18" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="F18" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="G18" t="s">
         <v>42</v>
       </c>
+      <c r="H18">
+        <v>16</v>
+      </c>
       <c r="I18" t="s">
         <v>37</v>
       </c>
@@ -1610,7 +1714,10 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="3:13">
+    <row r="19" spans="2:13">
+      <c r="B19">
+        <v>17</v>
+      </c>
       <c r="C19" t="s">
         <v>17</v>
       </c>
@@ -1620,9 +1727,15 @@
       <c r="E19" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="F19" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="G19" t="s">
         <v>42</v>
       </c>
+      <c r="H19">
+        <v>17</v>
+      </c>
       <c r="I19" t="s">
         <v>38</v>
       </c>
@@ -1632,11 +1745,17 @@
       <c r="K19" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="L19" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="M19" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="3:13">
+    <row r="20" spans="2:13">
+      <c r="B20">
+        <v>18</v>
+      </c>
       <c r="C20" t="s">
         <v>18</v>
       </c>
@@ -1646,9 +1765,15 @@
       <c r="E20" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="F20" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="G20" t="s">
         <v>42</v>
       </c>
+      <c r="H20">
+        <v>18</v>
+      </c>
       <c r="I20" t="s">
         <v>39</v>
       </c>
@@ -1658,18 +1783,27 @@
       <c r="K20" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="L20" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="M20" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="3:13">
+    <row r="21" spans="2:13">
+      <c r="B21">
+        <v>19</v>
+      </c>
       <c r="C21" t="s">
         <v>0</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" t="s">
-        <v>115</v>
+        <v>111</v>
+      </c>
+      <c r="H21">
+        <v>19</v>
       </c>
       <c r="I21" t="s">
         <v>40</v>
@@ -1680,22 +1814,25 @@
       <c r="K21" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="L21" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="M21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="3:13">
+    <row r="24" spans="2:13">
       <c r="D24" s="16" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="3:13" ht="181.5" customHeight="1">
+    <row r="25" spans="2:13" ht="181.5" customHeight="1">
       <c r="D25" s="11"/>
     </row>
-    <row r="26" spans="3:13" ht="16.5" thickBot="1">
+    <row r="26" spans="2:13" ht="16.5" thickBot="1">
       <c r="D26" s="5"/>
     </row>
-    <row r="27" spans="3:13" ht="86.25" thickBot="1">
+    <row r="27" spans="2:13" ht="86.25" thickBot="1">
       <c r="D27" s="12" t="s">
         <v>65</v>
       </c>
@@ -1709,7 +1846,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="3:13" ht="15.75" thickBot="1">
+    <row r="28" spans="2:13" ht="15.75" thickBot="1">
       <c r="D28" s="7">
         <v>1</v>
       </c>
@@ -1723,7 +1860,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="3:13" ht="15.75" thickBot="1">
+    <row r="29" spans="2:13" ht="15.75" thickBot="1">
       <c r="D29" s="8">
         <v>3</v>
       </c>
@@ -1737,7 +1874,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="3:13" ht="15.75" thickBot="1">
+    <row r="30" spans="2:13" ht="15.75" thickBot="1">
       <c r="D30" s="7">
         <v>2</v>
       </c>
@@ -1751,7 +1888,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="3:13" ht="15.75" thickBot="1">
+    <row r="31" spans="2:13" ht="15.75" thickBot="1">
       <c r="D31" s="8">
         <v>4</v>
       </c>
@@ -1765,7 +1902,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="3:13" ht="15.75" thickBot="1">
+    <row r="32" spans="2:13" ht="15.75" thickBot="1">
       <c r="D32" s="7">
         <v>6</v>
       </c>

</xml_diff>